<commit_message>
aggiunge grassetto titolo tabella
</commit_message>
<xml_diff>
--- a/M.1 - Introduzione all'ethical hacking/W.4/03.15/esercizio round Robin Svolto.xlsx
+++ b/M.1 - Introduzione all'ethical hacking/W.4/03.15/esercizio round Robin Svolto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\NewProject\M.1 - Introduzione all'ethical hacking\W.4\03.15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455113FD-CA12-4D13-A05B-D975A04DEDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3F3593-1DDF-4DA7-AADD-B9B0DCFA1080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1BE84015-90A1-4549-8AA2-5809278197E7}"/>
   </bookViews>
@@ -273,15 +273,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <font>
+        <b/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -364,6 +367,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -371,15 +383,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -399,7 +402,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{17D9438D-34AE-4BBF-8187-21EB18AB9482}" name="Tabella1" displayName="Tabella1" ref="C5:E10" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{17D9438D-34AE-4BBF-8187-21EB18AB9482}" name="Tabella1" displayName="Tabella1" ref="C5:E10" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="C5:E10" xr:uid="{17D9438D-34AE-4BBF-8187-21EB18AB9482}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:E10">
     <sortCondition ref="D5:D10"/>
@@ -713,7 +716,7 @@
   <dimension ref="B5:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,13 +728,13 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1000,19 +1003,19 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1030,11 +1033,11 @@
         <v>26</v>
       </c>
       <c r="F34" s="2">
-        <f>E34-C34</f>
+        <f t="shared" ref="F34:G38" si="0">E34-C34</f>
         <v>26</v>
       </c>
       <c r="G34" s="2">
-        <f>F34-D34</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -1052,11 +1055,11 @@
         <v>102</v>
       </c>
       <c r="F35" s="2">
-        <f>E35-C35</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="G35" s="2">
-        <f>F35-D35</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
@@ -1074,11 +1077,11 @@
         <v>122</v>
       </c>
       <c r="F36" s="2">
-        <f>E36-C36</f>
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="G36" s="2">
-        <f>F36-D36</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
@@ -1096,11 +1099,11 @@
         <v>124</v>
       </c>
       <c r="F37" s="2">
-        <f>E37-C37</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="G37" s="2">
-        <f>F37-D37</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -1118,11 +1121,11 @@
         <v>106</v>
       </c>
       <c r="F38" s="2">
-        <f>E38-C38</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="G38" s="2">
-        <f>F38-D38</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>

</xml_diff>